<commit_message>
Checkpoint from VS Code for cloud agent session
</commit_message>
<xml_diff>
--- a/Putt Allotment.xlsx
+++ b/Putt Allotment.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,21 @@
           <t>STATUS</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>REMINDER_ROW_ID</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>REMINDER_SNOOZE_UNTIL</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>REMINDER_DISMISSED</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -553,6 +568,15 @@
         <is>
           <t>WAITING</t>
         </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>11b46c4e-084f-42b1-acd9-7a800fb62cf4</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -597,6 +621,15 @@
           <t>WAITING</t>
         </is>
       </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>d5caa7d8-6422-4365-ba4c-6033a58cf91a</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -640,6 +673,15 @@
           <t>WAITING</t>
         </is>
       </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>4b013cf0-75ea-4221-bc28-0d683724c08a</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -683,6 +725,15 @@
           <t>WAITING</t>
         </is>
       </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>ba135f90-2877-472c-b0af-fffbab774325</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -725,6 +776,15 @@
         <is>
           <t>WAITING</t>
         </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>77bb20c2-2f4a-43fe-9275-a10bde9b17f9</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 15-minute reminder system with snooze/dismiss functionality
</commit_message>
<xml_diff>
--- a/Putt Allotment.xlsx
+++ b/Putt Allotment.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,11 @@
           <t>STATUS</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>REMINDER_ROW_ID</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -552,6 +557,11 @@
       <c r="M2" t="inlineStr">
         <is>
           <t>WAITING</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>4d7c1477-3f86-45d5-80e3-f0b872efcc6c</t>
         </is>
       </c>
     </row>
@@ -597,6 +607,11 @@
           <t>WAITING</t>
         </is>
       </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>b6ea6898-1d75-408e-9d13-7d68e0a9c46a</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -640,6 +655,11 @@
           <t>WAITING</t>
         </is>
       </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>353e5b8d-8c30-4ada-a163-02abba498742</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -683,6 +703,11 @@
           <t>WAITING</t>
         </is>
       </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>dc53b0ae-f468-4454-9216-44dd95cf90d6</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -724,6 +749,11 @@
       <c r="M6" t="inlineStr">
         <is>
           <t>WAITING</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>182d2127-3809-4a2e-bba0-aae36013aa1f</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: improve debug display for time_blocks in session_state
</commit_message>
<xml_diff>
--- a/Putt Allotment.xlsx
+++ b/Putt Allotment.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Meta" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +505,41 @@
           <t>REMINDER_ROW_ID</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Patient ID</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>REMINDER_SNOOZE_UNTIL</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>REMINDER_DISMISSED</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>STATUS_CHANGED_AT</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>ACTUAL_START_AT</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>ACTUAL_END_AT</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>STATUS_LOG</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -564,6 +600,15 @@
           <t>4d7c1477-3f86-45d5-80e3-f0b872efcc6c</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -612,6 +657,15 @@
           <t>b6ea6898-1d75-408e-9d13-7d68e0a9c46a</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -660,6 +714,15 @@
           <t>353e5b8d-8c30-4ada-a163-02abba498742</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -708,6 +771,15 @@
           <t>dc53b0ae-f468-4454-9216-44dd95cf90d6</t>
         </is>
       </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -754,6 +826,70 @@
       <c r="N6" t="inlineStr">
         <is>
           <t>182d2127-3809-4a2e-bba0-aae36013aa1f</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>key</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>time_blocks</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>[{"assistant": "BABU", "date": "2025-12-27", "reason": "Backend Work", "start_time": "20:46", "end_time": "20:50"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>time_blocks_updated_at</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-27T02:24:24.675570+05:30</t>
         </is>
       </c>
     </row>

</xml_diff>